<commit_message>
Updated on 30 Aug 2017
</commit_message>
<xml_diff>
--- a/horizon/xl_templates/48006_new_asldfkj_alsdnvla.xlsx
+++ b/horizon/xl_templates/48006_new_asldfkj_alsdnvla.xlsx
@@ -22,13 +22,13 @@
     <t>V</t>
   </si>
   <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>KG</t>
-  </si>
-  <si>
-    <t>Trip</t>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>Q2 (Ton)</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>

</xml_diff>